<commit_message>
Added the virtual taps
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/example_transformer_tpe.xlsx
+++ b/Grids_and_profiles/grids/example_transformer_tpe.xlsx
@@ -1,33 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\GridCal\Grids_and_profiles\grids\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="6975" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="config" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bus" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="branch" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="load" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="static_generator" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="battery" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="controlled_generator" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="shunt" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="wires" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="overhead_line_types" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="underground_cable_types" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sequence_line_types" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="transformer_types" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="config" sheetId="1" r:id="rId1"/>
+    <sheet name="bus" sheetId="2" r:id="rId2"/>
+    <sheet name="branch" sheetId="3" r:id="rId3"/>
+    <sheet name="load" sheetId="4" r:id="rId4"/>
+    <sheet name="static_generator" sheetId="5" r:id="rId5"/>
+    <sheet name="battery" sheetId="6" r:id="rId6"/>
+    <sheet name="controlled_generator" sheetId="7" r:id="rId7"/>
+    <sheet name="shunt" sheetId="8" r:id="rId8"/>
+    <sheet name="wires" sheetId="9" r:id="rId9"/>
+    <sheet name="overhead_line_types" sheetId="10" r:id="rId10"/>
+    <sheet name="underground_cable_types" sheetId="11" r:id="rId11"/>
+    <sheet name="sequence_line_types" sheetId="12" r:id="rId12"/>
+    <sheet name="transformer_types" sheetId="13" r:id="rId13"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="116">
   <si>
     <t>Property</t>
   </si>
@@ -191,9 +195,6 @@
     <t>branch_type</t>
   </si>
   <si>
-    <t>type_obj</t>
-  </si>
-  <si>
     <t>Branch 1</t>
   </si>
   <si>
@@ -375,28 +376,32 @@
   </si>
   <si>
     <t>Short_circuit_voltage</t>
+  </si>
+  <si>
+    <t>template</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -411,26 +416,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -718,20 +740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -739,30 +755,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -772,116 +788,97 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -898,112 +895,100 @@
         <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>108</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="n">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="n">
+        <v>63</v>
+      </c>
+      <c r="C2">
         <v>66</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>11</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>0.8</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0.1</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>0.1</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1047,8 +1032,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -1094,8 +1079,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1141,8 +1126,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1189,25 +1174,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1254,15 +1235,15 @@
         <v>53</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -1274,48 +1255,48 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
         <v>56</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
         <v>57</v>
       </c>
-      <c r="H2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>58</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>59</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>60</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>61</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" t="s">
         <v>62</v>
       </c>
-      <c r="N2" t="s">
-        <v>62</v>
-      </c>
-      <c r="O2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="1" t="n">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -1327,79 +1308,73 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" t="s">
         <v>65</v>
       </c>
-      <c r="G3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>66</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>67</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" t="s">
         <v>68</v>
       </c>
-      <c r="L3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>69</v>
       </c>
-      <c r="Q3" t="s">
-        <v>70</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>44</v>
@@ -1408,12 +1383,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
@@ -1428,46 +1403,40 @@
         <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" t="n">
+        <v>75</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>44</v>
@@ -1477,63 +1446,57 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>44</v>
@@ -1542,76 +1505,70 @@
         <v>45</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>91</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>44</v>
@@ -1620,12 +1577,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -1633,71 +1590,65 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>9999</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>-9999</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>9999</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>9999</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>1</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>0</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>44</v>
@@ -1707,39 +1658,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed (see issue #93)
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/example_transformer_tpe.xlsx
+++ b/Grids_and_profiles/grids/example_transformer_tpe.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\GridCal\Grids_and_profiles\grids\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michel\gits\gridcal\GridCal\Grids_and_profiles\grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C822874F-D7EE-441C-B651-F2C4FA52A4B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="6975" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="6975" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -357,34 +358,34 @@
     <t>B0</t>
   </si>
   <si>
-    <t>HV_nominal_voltage</t>
-  </si>
-  <si>
-    <t>LV_nominal_voltage</t>
-  </si>
-  <si>
-    <t>Nominal_power</t>
-  </si>
-  <si>
-    <t>Copper_losses</t>
-  </si>
-  <si>
-    <t>Iron_losses</t>
-  </si>
-  <si>
-    <t>No_load_current</t>
-  </si>
-  <si>
-    <t>Short_circuit_voltage</t>
-  </si>
-  <si>
     <t>template</t>
+  </si>
+  <si>
+    <t>HV</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>Pcu</t>
+  </si>
+  <si>
+    <t>Pfe</t>
+  </si>
+  <si>
+    <t>I0</t>
+  </si>
+  <si>
+    <t>Vsc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -740,12 +741,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -802,12 +803,12 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -853,12 +854,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -871,12 +872,12 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -913,37 +914,48 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -981,12 +993,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1179,14 +1191,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1235,7 +1264,7 @@
         <v>53</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1350,12 +1379,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1418,12 +1447,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1451,12 +1480,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1526,12 +1555,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1630,12 +1659,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -1663,12 +1692,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">

</xml_diff>